<commit_message>
Minor updates in Danger, Separation and class diagram + updated
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mette\Documents\4. Semester\SWT_Gruppe21_ATM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris W Olesen\Documents\6.semester\SWT\SWT_ATM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C6C8258-D1F4-4B7F-9358-701D2C75E5EA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE88C139-E0D1-4E19-B966-260CBD9FBF7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{C49E8341-C52A-4BC8-BBCA-626CF73636D2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Track test!</t>
+  </si>
+  <si>
+    <t>Separation - calculateDistantance test</t>
   </si>
 </sst>
 </file>
@@ -166,12 +169,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Kontrollér celle" xfId="2" builtinId="23"/>
@@ -194,7 +198,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kontor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -232,7 +236,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kontor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -338,7 +342,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kontor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -488,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8317FA0-267C-4D18-B8C8-8D9465CE989D}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,18 +540,18 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -571,6 +575,14 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tasks updated, Alarm updated
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris W Olesen\Documents\6.semester\SWT\SWT_ATM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mikkel\Desktop\AU\4. Semester\GIT\SWT_Gruppe21_ATM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE88C139-E0D1-4E19-B966-260CBD9FBF7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{C49E8341-C52A-4BC8-BBCA-626CF73636D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +72,15 @@
   </si>
   <si>
     <t>Separation - calculateDistantance test</t>
+  </si>
+  <si>
+    <t>Mikkel</t>
+  </si>
+  <si>
+    <t>raiseAlaram()</t>
+  </si>
+  <si>
+    <t>deactivateAlarm()</t>
   </si>
 </sst>
 </file>
@@ -110,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +145,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -169,13 +183,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Kontrollér celle" xfId="2" builtinId="23"/>
@@ -495,7 +510,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +589,22 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+    </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Updated task and added calculations
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chris W Olesen\Documents\6.semester\SWT\SWT_ATM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D7D6453F-BEA6-494D-BC8B-6DFE676A360C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{1D0431B7-1065-48F4-A316-1D0AEE3324FD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{C49E8341-C52A-4BC8-BBCA-626CF73636D2}"/>
   </bookViews>
@@ -514,7 +514,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,10 +610,10 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>